<commit_message>
Films up to Guardians 2 finished
</commit_message>
<xml_diff>
--- a/Guide.xlsx
+++ b/Guide.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://leeds365-my.sharepoint.com/personal/medbcoo_leeds_ac_uk/Documents/Ultron/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="486" documentId="8_{A6858830-BA2B-474A-BF48-2332F5FF8DCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F1B940E3-AB5A-4FA8-A5A9-56D53BFF5CFE}"/>
+  <xr:revisionPtr revIDLastSave="893" documentId="8_{A6858830-BA2B-474A-BF48-2332F5FF8DCB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{99C21B77-3377-45EE-8EF2-AA57C9A34B70}"/>
   <bookViews>
-    <workbookView xWindow="-20520" yWindow="1695" windowWidth="20640" windowHeight="11160" xr2:uid="{6990565D-D1EF-4827-9BF5-092520955A52}"/>
+    <workbookView xWindow="-20520" yWindow="1695" windowWidth="20640" windowHeight="11160" activeTab="2" xr2:uid="{6990565D-D1EF-4827-9BF5-092520955A52}"/>
   </bookViews>
   <sheets>
     <sheet name="Films" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="158">
   <si>
     <t>Iron Man</t>
   </si>
@@ -205,9 +205,6 @@
     <t>Villain defeated</t>
   </si>
   <si>
-    <t>Someone says "Vibranium"</t>
-  </si>
-  <si>
     <t>A previously unmentioned use for vibranium is revealed.</t>
   </si>
   <si>
@@ -245,13 +242,280 @@
   </si>
   <si>
     <t>New character with "foreign" accent</t>
+  </si>
+  <si>
+    <t>Anyone says "Ultron"</t>
+  </si>
+  <si>
+    <t>Anyone says "Avengers"</t>
+  </si>
+  <si>
+    <t>Anyone mentions “bad language”</t>
+  </si>
+  <si>
+    <t>Mjolnir moves slighty</t>
+  </si>
+  <si>
+    <t>Slow motion</t>
+  </si>
+  <si>
+    <t>SLOWMO</t>
+  </si>
+  <si>
+    <t>Ant-man changes size</t>
+  </si>
+  <si>
+    <t>ANTMAN</t>
+  </si>
+  <si>
+    <t>Hulk and Black Widow sexual tension</t>
+  </si>
+  <si>
+    <t>Infinity stones are seen or referenced</t>
+  </si>
+  <si>
+    <t>Vision awakens</t>
+  </si>
+  <si>
+    <t>Quicksilver dies</t>
+  </si>
+  <si>
+    <t>Bug or size pun</t>
+  </si>
+  <si>
+    <t>Scott says he no longer steals</t>
+  </si>
+  <si>
+    <t>A lock is entered or broken (This includes jumping through the hole itself)</t>
+  </si>
+  <si>
+    <t>The words "Ant-Man" and "Yellow Jacket" are said</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tea or Waffles are shown </t>
+  </si>
+  <si>
+    <t>See a new type of ant</t>
+  </si>
+  <si>
+    <t>EVERY</t>
+  </si>
+  <si>
+    <t>The words "Quantum", "Lab" or "House" are said</t>
+  </si>
+  <si>
+    <t>Germany is referenced</t>
+  </si>
+  <si>
+    <t>The police show up or are pursuing them</t>
+  </si>
+  <si>
+    <t>Scott is "possessed"</t>
+  </si>
+  <si>
+    <t>Scott becomes giant</t>
+  </si>
+  <si>
+    <t>"Oh my god! They were evil!?"</t>
+  </si>
+  <si>
+    <t>TWIST</t>
+  </si>
+  <si>
+    <t>CROSSOVER</t>
+  </si>
+  <si>
+    <t>Avenger not named in title appears</t>
+  </si>
+  <si>
+    <t>Someone says "Vibranium" or "Wakanda"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A suit does an energy blast </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A spear is extended </t>
+  </si>
+  <si>
+    <t>There is a flashback or someone travels to the ancestor realm</t>
+  </si>
+  <si>
+    <t>We find out who Killmonger really is</t>
+  </si>
+  <si>
+    <t>See the heart-shaped herb</t>
+  </si>
+  <si>
+    <t>"Wakanda Forever!"</t>
+  </si>
+  <si>
+    <t>Any reference to Hitler or the Nazis</t>
+  </si>
+  <si>
+    <t>Steve gets shredded</t>
+  </si>
+  <si>
+    <t>Someone mentions Brooklyn</t>
+  </si>
+  <si>
+    <t>Captain America throws his Shield</t>
+  </si>
+  <si>
+    <t>Red Skull reveals his red skull</t>
+  </si>
+  <si>
+    <t>Heavy-handed "Girl Power" scene</t>
+  </si>
+  <si>
+    <t>Someone makes a pop culture reference</t>
+  </si>
+  <si>
+    <t>Someone banters with their suit's artificial intelligence</t>
+  </si>
+  <si>
+    <t>Spider-Man introduced</t>
+  </si>
+  <si>
+    <t>Someone forced to chose between protecting/obtaining an Infinity Stone and someone else's life.</t>
+  </si>
+  <si>
+    <t>Steve lifts Mjolnir</t>
+  </si>
+  <si>
+    <t>Thanos uses an infinity stone</t>
+  </si>
+  <si>
+    <t>The Snap</t>
+  </si>
+  <si>
+    <t>Anyone talks about trust</t>
+  </si>
+  <si>
+    <t>Glass shatters</t>
+  </si>
+  <si>
+    <t>Bucky catches Cap's shield</t>
+  </si>
+  <si>
+    <t>Someone previously thought dead is shown to be alive</t>
+  </si>
+  <si>
+    <t>Anyone says "freedom", "order" or "chaos"</t>
+  </si>
+  <si>
+    <t>That cool knife switch in the fight between bucky and cap</t>
+  </si>
+  <si>
+    <t>"Puny God"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The words "Lawson", "Pegasus" or "Skroll" are said </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A misogynistic comment is made </t>
+  </si>
+  <si>
+    <t>A 90's reference is made</t>
+  </si>
+  <si>
+    <t>We find out how Fury lost his eye</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A Skroll changes its form </t>
+  </si>
+  <si>
+    <t>"Avengers" or "Winter Soldier" said</t>
+  </si>
+  <si>
+    <t>Location title shown</t>
+  </si>
+  <si>
+    <t>Someone goes through a wall of a building</t>
+  </si>
+  <si>
+    <t>Someone appears with a black eye</t>
+  </si>
+  <si>
+    <t>Who killed Stark's parents?</t>
+  </si>
+  <si>
+    <t>AVENGER</t>
+  </si>
+  <si>
+    <t>Each pick a hero and drink every time they use their powers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The words "Dark Dimension", "Ancient One" or "Astral Body" are said </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strange corrects someone that he is indeed a doctor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The cape saves Strange </t>
+  </si>
+  <si>
+    <t>Acid trip visuals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The mirror dimension appears </t>
+  </si>
+  <si>
+    <t>Orange sparky chains!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strange scales Everest? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The words "Avengers", "Thanos", "Stones" or "Time" are said </t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is a location or year title onscreen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">An Avenger runs into their prior self, spouse or parent while traveling time </t>
+  </si>
+  <si>
+    <t xml:space="preserve">A stone is obtained </t>
+  </si>
+  <si>
+    <t>An Avenger dies</t>
+  </si>
+  <si>
+    <t>Drax takes a comment or action literally</t>
+  </si>
+  <si>
+    <t>Yondu whistles his arrow around</t>
+  </si>
+  <si>
+    <t>Someone doesn't know who Star Lord is</t>
+  </si>
+  <si>
+    <t>"I am Groot"</t>
+  </si>
+  <si>
+    <t>"They got my dick message!"</t>
+  </si>
+  <si>
+    <t>"Thanos" or "Orb" is said</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The words "Star Lord", "Battery" or "Dad" are said </t>
+  </si>
+  <si>
+    <t>Drax laughs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New planet/location shown </t>
+  </si>
+  <si>
+    <t>"I'm Mary Poppins y'all!"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,6 +528,12 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -633,16 +903,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F63F8968-FA48-4997-A236-6B74290AF4B4}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" customWidth="1"/>
-    <col min="2" max="2" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -664,10 +934,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
         <v>27</v>
@@ -675,21 +945,21 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>
@@ -697,94 +967,178 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -792,7 +1146,7 @@
         <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>97</v>
       </c>
       <c r="C21" t="s">
         <v>27</v>
@@ -803,7 +1157,7 @@
         <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C22" t="s">
         <v>26</v>
@@ -813,38 +1167,711 @@
       <c r="A23" t="s">
         <v>16</v>
       </c>
+      <c r="B23" t="s">
+        <v>98</v>
+      </c>
+      <c r="C23" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>16</v>
       </c>
+      <c r="B24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>16</v>
       </c>
+      <c r="B25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="B26" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="B27" t="s">
+        <v>102</v>
+      </c>
+      <c r="C27" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>19</v>
+        <v>16</v>
+      </c>
+      <c r="B28" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" t="s">
+        <v>104</v>
+      </c>
+      <c r="C29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>105</v>
+      </c>
+      <c r="C30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
+        <v>106</v>
+      </c>
+      <c r="C31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" t="s">
+        <v>107</v>
+      </c>
+      <c r="C32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" t="s">
+        <v>117</v>
+      </c>
+      <c r="C34" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" t="s">
+        <v>118</v>
+      </c>
+      <c r="C35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" t="s">
+        <v>119</v>
+      </c>
+      <c r="C36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" t="s">
+        <v>120</v>
+      </c>
+      <c r="C37" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" t="s">
+        <v>121</v>
+      </c>
+      <c r="C38" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" t="s">
+        <v>122</v>
+      </c>
+      <c r="C39" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" t="s">
+        <v>124</v>
+      </c>
+      <c r="C40" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" t="s">
+        <v>125</v>
+      </c>
+      <c r="C41" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42" t="s">
+        <v>126</v>
+      </c>
+      <c r="C42" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" t="s">
+        <v>128</v>
+      </c>
+      <c r="C43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" t="s">
+        <v>127</v>
+      </c>
+      <c r="C44" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45" t="s">
+        <v>112</v>
+      </c>
+      <c r="C45" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" t="s">
+        <v>129</v>
+      </c>
+      <c r="C46" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" t="s">
+        <v>130</v>
+      </c>
+      <c r="C47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" t="s">
+        <v>131</v>
+      </c>
+      <c r="C48" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" t="s">
+        <v>132</v>
+      </c>
+      <c r="C49" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>12</v>
+      </c>
+      <c r="B50" t="s">
+        <v>133</v>
+      </c>
+      <c r="C50" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>13</v>
+      </c>
+      <c r="B51" t="s">
+        <v>136</v>
+      </c>
+      <c r="C51" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>13</v>
+      </c>
+      <c r="B52" t="s">
+        <v>137</v>
+      </c>
+      <c r="C52" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>13</v>
+      </c>
+      <c r="B53" t="s">
+        <v>138</v>
+      </c>
+      <c r="C53" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>13</v>
+      </c>
+      <c r="B54" t="s">
+        <v>139</v>
+      </c>
+      <c r="C54" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>13</v>
+      </c>
+      <c r="B55" t="s">
+        <v>140</v>
+      </c>
+      <c r="C55" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>13</v>
+      </c>
+      <c r="B56" t="s">
+        <v>141</v>
+      </c>
+      <c r="C56" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>13</v>
+      </c>
+      <c r="B57" t="s">
+        <v>142</v>
+      </c>
+      <c r="C57" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>20</v>
       </c>
+      <c r="B58" t="s">
+        <v>109</v>
+      </c>
+      <c r="C58" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>20</v>
+      </c>
+      <c r="B59" t="s">
+        <v>114</v>
+      </c>
+      <c r="C59" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>20</v>
+      </c>
+      <c r="B60" t="s">
+        <v>143</v>
+      </c>
+      <c r="C60" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>20</v>
+      </c>
+      <c r="B61" t="s">
+        <v>144</v>
+      </c>
+      <c r="C61" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>20</v>
+      </c>
+      <c r="B62" t="s">
+        <v>145</v>
+      </c>
+      <c r="C62" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>20</v>
+      </c>
+      <c r="B63" t="s">
+        <v>146</v>
+      </c>
+      <c r="C63" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>20</v>
+      </c>
+      <c r="B64" t="s">
+        <v>147</v>
+      </c>
+      <c r="C64" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>9</v>
+      </c>
+      <c r="B65" t="s">
+        <v>148</v>
+      </c>
+      <c r="C65" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>9</v>
+      </c>
+      <c r="B66" t="s">
+        <v>149</v>
+      </c>
+      <c r="C66" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>9</v>
+      </c>
+      <c r="B67" t="s">
+        <v>150</v>
+      </c>
+      <c r="C67" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>9</v>
+      </c>
+      <c r="B68" t="s">
+        <v>151</v>
+      </c>
+      <c r="C68" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>9</v>
+      </c>
+      <c r="B69" t="s">
+        <v>152</v>
+      </c>
+      <c r="C69" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>9</v>
+      </c>
+      <c r="B70" t="s">
+        <v>153</v>
+      </c>
+      <c r="C70" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>14</v>
+      </c>
+      <c r="B71" t="s">
+        <v>154</v>
+      </c>
+      <c r="C71" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>14</v>
+      </c>
+      <c r="B72" t="s">
+        <v>155</v>
+      </c>
+      <c r="C72" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>14</v>
+      </c>
+      <c r="B73" t="s">
+        <v>156</v>
+      </c>
+      <c r="C73" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>14</v>
+      </c>
+      <c r="B74" t="s">
+        <v>157</v>
+      </c>
+      <c r="C74" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>17</v>
+      </c>
+      <c r="B75" t="s">
+        <v>113</v>
+      </c>
+      <c r="C75" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>115</v>
+      </c>
+      <c r="C76" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>116</v>
+      </c>
+      <c r="C77" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>0</v>
+      </c>
+      <c r="B78" t="s">
+        <v>46</v>
+      </c>
+      <c r="C78" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>0</v>
+      </c>
+      <c r="B79" t="s">
+        <v>23</v>
+      </c>
+      <c r="C79" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>0</v>
+      </c>
+      <c r="B80" t="s">
+        <v>47</v>
+      </c>
+      <c r="C80" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>0</v>
+      </c>
+      <c r="B81" t="s">
+        <v>49</v>
+      </c>
+      <c r="C81" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>0</v>
+      </c>
+      <c r="B82" t="s">
+        <v>54</v>
+      </c>
+      <c r="C82" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>6</v>
+      </c>
+      <c r="B85" t="s">
+        <v>111</v>
+      </c>
+      <c r="C85" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>5</v>
+      </c>
+      <c r="B87" t="s">
+        <v>110</v>
+      </c>
+      <c r="C87" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>123</v>
+      </c>
+      <c r="C88" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C82">
+    <sortCondition ref="A2:A82"/>
+  </sortState>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -852,10 +1879,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA42F67-A9E1-45A0-916A-61B04FD08D72}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,6 +1928,9 @@
       <c r="A4" t="s">
         <v>29</v>
       </c>
+      <c r="B4" t="s">
+        <v>87</v>
+      </c>
       <c r="C4" t="s">
         <v>27</v>
       </c>
@@ -909,8 +1939,11 @@
       <c r="A5" t="s">
         <v>30</v>
       </c>
+      <c r="B5" t="s">
+        <v>87</v>
+      </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1005,13 +2038,19 @@
       <c r="A14" t="s">
         <v>55</v>
       </c>
+      <c r="B14" t="s">
+        <v>87</v>
+      </c>
       <c r="C14" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="B15" t="s">
+        <v>87</v>
       </c>
       <c r="C15" t="s">
         <v>27</v>
@@ -1019,10 +2058,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" t="s">
         <v>59</v>
-      </c>
-      <c r="B16" t="s">
-        <v>60</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
@@ -1030,10 +2069,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C17" t="s">
         <v>35</v>
@@ -1041,7 +2080,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="B18" t="s">
+        <v>87</v>
       </c>
       <c r="C18" t="s">
         <v>27</v>
@@ -1049,7 +2091,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+      <c r="B19" t="s">
+        <v>87</v>
       </c>
       <c r="C19" t="s">
         <v>35</v>
@@ -1057,10 +2102,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C20" t="s">
         <v>27</v>
@@ -1068,10 +2113,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C21" t="s">
         <v>26</v>
@@ -1079,9 +2124,67 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+      <c r="B22" t="s">
+        <v>87</v>
       </c>
       <c r="C22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>93</v>
+      </c>
+      <c r="B25" t="s">
+        <v>94</v>
+      </c>
+      <c r="C25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" t="s">
+        <v>95</v>
+      </c>
+      <c r="C26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>135</v>
+      </c>
+      <c r="B27" t="s">
+        <v>134</v>
+      </c>
+      <c r="C27" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1095,8 +2198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1114775-9AFC-4950-96C4-B081826015F1}">
   <dimension ref="A1:Z21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1104,11 +2207,23 @@
     <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.5703125" style="3" customWidth="1"/>
     <col min="3" max="3" width="5.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.140625" style="3" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" style="3" customWidth="1"/>
-    <col min="7" max="10" width="9.140625" style="3" customWidth="1"/>
-    <col min="11" max="26" width="9.140625" style="3"/>
+    <col min="7" max="7" width="7.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5703125" style="3" customWidth="1"/>
+    <col min="16" max="16" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.5703125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="11.5703125" style="3" customWidth="1"/>
+    <col min="19" max="19" width="9.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="26" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1143,22 +2258,32 @@
         <v>53</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="M1" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
+        <v>66</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>134</v>
+      </c>
       <c r="T1" s="2"/>
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
@@ -1210,6 +2335,21 @@
       <c r="N2" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="O2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1254,6 +2394,21 @@
       <c r="N3" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="O3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1298,6 +2453,21 @@
       <c r="N4" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="O4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1342,6 +2512,21 @@
       <c r="N5" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="O5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1386,6 +2571,21 @@
       <c r="N6" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="O6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1428,7 +2628,22 @@
         <v>32</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
@@ -1474,6 +2689,21 @@
       <c r="N8" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="O8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1518,6 +2748,21 @@
       <c r="N9" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="O9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S9" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1562,6 +2807,21 @@
       <c r="N10" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="O10" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S10" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1606,6 +2866,21 @@
       <c r="N11" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="O11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S11" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1650,6 +2925,21 @@
       <c r="N12" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="O12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="S12" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1694,6 +2984,21 @@
       <c r="N13" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="O13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S13" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1738,6 +3043,21 @@
       <c r="N14" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="O14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S14" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1782,6 +3102,21 @@
       <c r="N15" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="O15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="R15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S15" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1826,8 +3161,23 @@
       <c r="N16" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="S16" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1870,8 +3220,23 @@
       <c r="N17" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S17" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1914,8 +3279,23 @@
       <c r="N18" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O18" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="P18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S18" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1958,8 +3338,23 @@
       <c r="N19" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S19" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -2002,8 +3397,23 @@
       <c r="N20" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="R20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S20" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -2045,6 +3455,21 @@
       </c>
       <c r="N21" s="3" t="s">
         <v>32</v>
+      </c>
+      <c r="O21" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P21" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q21" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R21" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S21" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -2057,5 +3482,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>